<commit_message>
Added cost calculation to properties of heat exchanger object
</commit_message>
<xml_diff>
--- a/data/Jones_P3_PinCH_2.xlsx
+++ b/data/Jones_P3_PinCH_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>HEX</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>ExtremT</t>
+  </si>
+  <si>
+    <t>c_R</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,10 +1477,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,7 +1488,7 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1505,10 +1508,13 @@
         <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1528,10 +1534,13 @@
         <v>0.63</v>
       </c>
       <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2">
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1551,10 +1560,13 @@
         <v>0.63</v>
       </c>
       <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
         <v>313</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1574,10 +1586,13 @@
         <v>0.63</v>
       </c>
       <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
         <v>708</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1597,6 +1612,9 @@
         <v>0.63</v>
       </c>
       <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
         <v>505</v>
       </c>
     </row>
@@ -1757,9 +1775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added diverse tests and changed temperature calculation from the approach of Chen to the old
</commit_message>
<xml_diff>
--- a/data/Jones_P3_PinCH_2.xlsx
+++ b/data/Jones_P3_PinCH_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>HEX</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>c_R</t>
+  </si>
+  <si>
+    <t>OneMixerBool</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2375,11 +2378,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,9 +2391,10 @@
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2415,8 +2419,11 @@
       <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2440,6 +2447,9 @@
       </c>
       <c r="H2">
         <v>999999999999999</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added feasibility test for heat exchanger and corresponding unit tests
</commit_message>
<xml_diff>
--- a/data/Jones_P3_PinCH_2.xlsx
+++ b/data/Jones_P3_PinCH_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -1778,9 +1778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,7 +1867,7 @@
         <v>11500</v>
       </c>
       <c r="L2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1907,7 +1907,7 @@
         <v>7700</v>
       </c>
       <c r="L3">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>6400</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
         <v>7800</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2026,7 +2026,7 @@
         <v>3400</v>
       </c>
       <c r="L6" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M6" s="4">
         <v>0.08</v>
@@ -2068,7 +2068,7 @@
         <v>8400</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M7" s="1">
         <v>8.0000000000000002E-3</v>
@@ -2111,7 +2111,7 @@
         <v>12600</v>
       </c>
       <c r="L8" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N8" s="4"/>
     </row>
@@ -2152,7 +2152,7 @@
         <v>3500</v>
       </c>
       <c r="L9" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -2193,7 +2193,7 @@
         <v>5600</v>
       </c>
       <c r="L10" s="2">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -2234,7 +2234,7 @@
         <v>3600</v>
       </c>
       <c r="L11" s="2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -2274,7 +2274,7 @@
         <v>1800</v>
       </c>
       <c r="L12" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M12" s="4">
         <v>0.08</v>
@@ -2316,7 +2316,7 @@
         <v>8700</v>
       </c>
       <c r="L13" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M13" s="1">
         <v>8.0000000000000002E-3</v>
@@ -2380,7 +2380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>

</xml_diff>

<commit_message>
Added cost calculation (needs testing)
</commit_message>
<xml_diff>
--- a/data/Jones_P3_PinCH_2.xlsx
+++ b/data/Jones_P3_PinCH_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -561,9 +561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,9 +1778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,6 +2031,10 @@
       <c r="M6" s="4">
         <v>0.08</v>
       </c>
+      <c r="N6" s="4">
+        <f>K6*J6</f>
+        <v>15857600</v>
+      </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -2073,6 +2077,10 @@
       <c r="M7" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
+      <c r="N7" s="1">
+        <f>K7*J7</f>
+        <v>39177600</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2279,6 +2287,10 @@
       <c r="M12" s="4">
         <v>0.08</v>
       </c>
+      <c r="N12" s="4">
+        <f>K12*(J12-I12)</f>
+        <v>6004800</v>
+      </c>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2320,6 +2332,10 @@
       </c>
       <c r="M13" s="1">
         <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N13" s="1">
+        <f>K13*(J13-I13)</f>
+        <v>29023200</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added testing for split costs
</commit_message>
<xml_diff>
--- a/data/Jones_P3_PinCH_2.xlsx
+++ b/data/Jones_P3_PinCH_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -561,9 +561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U17" sqref="U17"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,9 +2396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented soft streams (needs testing)
</commit_message>
<xml_diff>
--- a/data/Jones_P3_PinCH_2.xlsx
+++ b/data/Jones_P3_PinCH_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>HEX</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>OneMixerBool</t>
+  </si>
+  <si>
+    <t>Soft</t>
   </si>
 </sst>
 </file>
@@ -273,12 +276,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1482,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1776,20 +1780,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1823,14 +1827,17 @@
       <c r="K1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1866,11 +1873,14 @@
         <f>ABS(D2-E2)*G2*H2</f>
         <v>11500</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1906,11 +1916,14 @@
         <f t="shared" ref="K3:K5" si="0">ABS(D3-E3)*G3*H3</f>
         <v>7700</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1946,11 +1959,14 @@
         <f t="shared" si="0"/>
         <v>6400</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1986,11 +2002,14 @@
         <f t="shared" si="0"/>
         <v>7800</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -2028,15 +2047,18 @@
       <c r="L6" s="2">
         <v>0</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
         <v>0.08</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <f>K6*J6</f>
         <v>15857600</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -2072,17 +2094,20 @@
         <v>8400</v>
       </c>
       <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
         <v>100</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <f>K7*J7</f>
         <v>39177600</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2121,9 +2146,12 @@
       <c r="L8" s="2">
         <v>0</v>
       </c>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2162,9 +2190,12 @@
       <c r="L9" s="2">
         <v>0</v>
       </c>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2201,11 +2232,14 @@
         <v>5600</v>
       </c>
       <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
         <v>400</v>
       </c>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2242,11 +2276,14 @@
         <v>3600</v>
       </c>
       <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
         <v>200</v>
       </c>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -2284,15 +2321,18 @@
       <c r="L12" s="2">
         <v>0</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
         <v>0.08</v>
       </c>
-      <c r="N12" s="4">
+      <c r="O12" s="4">
         <f>K12*(J12-I12)</f>
         <v>6004800</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -2327,28 +2367,62 @@
       <c r="K13" s="1">
         <v>8700</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
         <v>100</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <f>K13*(J13-I13)</f>
         <v>29023200</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
-    </row>
-    <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="12:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="12:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L24" s="4"/>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>

</xml_diff>